<commit_message>
Noted 2 doctoral theses, but couldn't calculate effect sizes; fixed README issues
</commit_message>
<xml_diff>
--- a/coded_effect_sizes.xlsx
+++ b/coded_effect_sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srivinay Tummarakota\Documents\VinaysDocs\Unboxing Politics\Books in the Home\books-in-the-home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31000ABB-D97E-4922-8303-372855A2258D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850CAE64-460A-4700-8F70-281D1FB7AA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59D706DF-03B4-44DD-A8EB-B27C936E1AA0}"/>
   </bookViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D899D00-894E-47DA-964E-FA933B438F9C}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>